<commit_message>
Getting ready for RCQ
</commit_message>
<xml_diff>
--- a/izzetChicken.xlsx
+++ b/izzetChicken.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D07A72-7C15-486C-9410-966FEED1A4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901277AD-ED45-4415-A9D4-F96D7BF17980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -143,12 +143,6 @@
     <t>Khans of Tarkir</t>
   </si>
   <si>
-    <t>Abrade</t>
-  </si>
-  <si>
-    <t>Hour of Devastation</t>
-  </si>
-  <si>
     <t>Flame-Blessed Bolt</t>
   </si>
   <si>
@@ -174,6 +168,15 @@
   </si>
   <si>
     <t>Amonkhet</t>
+  </si>
+  <si>
+    <t>Negate</t>
+  </si>
+  <si>
+    <t>Magic 2013</t>
+  </si>
+  <si>
+    <t>Magic 2014</t>
   </si>
 </sst>
 </file>
@@ -529,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +580,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F25" si="0">D2*E2</f>
+        <f t="shared" ref="F2:F26" si="0">D2*E2</f>
         <v>12.72</v>
       </c>
     </row>
@@ -932,14 +935,14 @@
         <v>7</v>
       </c>
       <c r="D19" s="3">
-        <v>0.17</v>
+        <v>0.09</v>
       </c>
       <c r="E19" s="2">
         <v>2</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
-        <v>0.34</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -947,104 +950,104 @@
         <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="3">
-        <v>0.09</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
-        <v>0.18</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="E21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="3">
-        <v>0.13</v>
+        <v>0.54</v>
       </c>
       <c r="E22" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
-        <v>0.26</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="3">
-        <v>0.54</v>
+        <v>0.78</v>
       </c>
       <c r="E23" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
-        <v>2.16</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="3">
-        <v>0.78</v>
+        <v>0.08</v>
       </c>
       <c r="E24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
-        <v>1.56</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1052,30 +1055,51 @@
         <v>45</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E26" s="2">
         <v>2</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="G25" s="3">
-        <f>SUM(F19:F25)</f>
-        <v>5.2200000000000006</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="3">
-        <f>SUM(F2:F25)</f>
-        <v>87.440000000000012</v>
+      <c r="G26" s="3">
+        <f>SUM(F19:F26)</f>
+        <v>5.0600000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="3">
+        <f>SUM(F2:F26)</f>
+        <v>87.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Brane gave me a Spikefield Hazard
</commit_message>
<xml_diff>
--- a/izzetChicken.xlsx
+++ b/izzetChicken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901277AD-ED45-4415-A9D4-F96D7BF17980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F85EE3-05F1-41A1-BA82-BD75176DEBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>Magic 2014</t>
+  </si>
+  <si>
+    <t>Spikefield Hazard: Spikefield Cave</t>
+  </si>
+  <si>
+    <t>Zendikar Rising</t>
   </si>
 </sst>
 </file>
@@ -532,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,14 +580,14 @@
         <v>7</v>
       </c>
       <c r="D2" s="3">
-        <v>3.18</v>
+        <v>2.97</v>
       </c>
       <c r="E2" s="2">
         <v>4</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F26" si="0">D2*E2</f>
-        <v>12.72</v>
+        <f t="shared" ref="F2:F27" si="0">D2*E2</f>
+        <v>11.88</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -595,14 +601,14 @@
         <v>7</v>
       </c>
       <c r="D3" s="3">
-        <v>0.17</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E3" s="2">
         <v>4</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>0.68</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -616,14 +622,14 @@
         <v>7</v>
       </c>
       <c r="D4" s="3">
-        <v>0.72</v>
+        <v>0.82</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
-        <v>2.88</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -658,14 +664,14 @@
         <v>7</v>
       </c>
       <c r="D6" s="3">
-        <v>4.79</v>
+        <v>4.46</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>4.79</v>
+        <v>4.46</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -679,14 +685,14 @@
         <v>7</v>
       </c>
       <c r="D7" s="3">
-        <v>0.26</v>
+        <v>0.3</v>
       </c>
       <c r="E7" s="2">
         <v>3</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
-        <v>0.78</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,14 +706,14 @@
         <v>7</v>
       </c>
       <c r="D8" s="3">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="E8" s="2">
         <v>3</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
-        <v>0.57000000000000006</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -721,14 +727,14 @@
         <v>7</v>
       </c>
       <c r="D9" s="3">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="E9" s="2">
         <v>3</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
-        <v>0.54</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -742,14 +748,14 @@
         <v>7</v>
       </c>
       <c r="D10" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.09</v>
       </c>
       <c r="E10" s="2">
         <v>4</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -784,14 +790,14 @@
         <v>7</v>
       </c>
       <c r="D12" s="3">
-        <v>2.78</v>
+        <v>3.14</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>2.78</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -805,249 +811,249 @@
         <v>7</v>
       </c>
       <c r="D13" s="3">
-        <v>0.98</v>
+        <v>1.06</v>
       </c>
       <c r="E13" s="2">
         <v>3</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
-        <v>2.94</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <v>14.88</v>
+        <v>0.37</v>
       </c>
       <c r="E14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
-        <v>29.76</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="3">
-        <v>1.8</v>
+        <v>13.84</v>
       </c>
       <c r="E15" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
-        <v>7.2</v>
+        <v>27.68</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="3">
-        <v>0.16</v>
+        <v>1.63</v>
       </c>
       <c r="E16" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>0.32</v>
+        <v>6.52</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="3">
-        <v>3.62</v>
+        <v>0.27</v>
       </c>
       <c r="E17" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="0"/>
-        <v>14.48</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="3">
-        <v>0.14000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="E18" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="0"/>
-        <v>0.42000000000000004</v>
-      </c>
-      <c r="G18" s="3">
-        <f>SUM(F2:F18)</f>
-        <v>82.22</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="3">
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
       <c r="E19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
-        <v>0.18</v>
+        <v>0.48</v>
+      </c>
+      <c r="G19" s="3">
+        <f>SUM(F2:F19)</f>
+        <v>80.290000000000006</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="3">
-        <v>0.13</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E21" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
-        <v>0.26</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="3">
-        <v>0.54</v>
+        <v>0.18</v>
       </c>
       <c r="E22" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
-        <v>2.16</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="3">
-        <v>0.78</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="2">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="0"/>
         <v>2</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>1.56</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="3">
-        <v>0.08</v>
+        <v>0.76</v>
       </c>
       <c r="E24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1055,51 +1061,72 @@
         <v>45</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="3">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="2">
         <v>2</v>
       </c>
-      <c r="F26" s="3">
-        <f t="shared" si="0"/>
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="G26" s="3">
-        <f>SUM(F19:F26)</f>
-        <v>5.0600000000000005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27" s="3">
-        <f>SUM(F2:F26)</f>
-        <v>87.28</v>
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="G27" s="3">
+        <f>SUM(F20:F27)</f>
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="3">
+        <f>SUM(F2:F27)</f>
+        <v>85.080000000000013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>